<commit_message>
Adjustment of File Names and Content
Added txt format "Reference List" and added the brand name for the datasheet's file name.
</commit_message>
<xml_diff>
--- a/Research Paper/RRL/Reference List.xlsx
+++ b/Research Paper/RRL/Reference List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://asiapacificcollege-my.sharepoint.com/personal/kpgeronimo_student_apc_edu_ph/Documents/ECEMETH/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keanu Geronimo\xzrn_\GitHub\ECE221-Group_B-Research\Research Paper\RRL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{59D33BFE-DBD2-4143-8A1D-01EDF8C23563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A542E69C-0692-4E1E-8F44-8EAAF584EF88}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DE6449-C69B-4F36-A739-997485FA7546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -142,25 +142,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -541,40 +538,40 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56" style="8" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="116.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56" style="6" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" customWidth="1"/>
+    <col min="5" max="5" width="19.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="116.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
@@ -586,21 +583,21 @@
       <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D3">
@@ -609,18 +606,18 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="345" x14ac:dyDescent="0.25">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D4">
@@ -632,55 +629,58 @@
       <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="7"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C5" s="5"/>
       <c r="E5"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="7"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C6" s="5"/>
       <c r="E6"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="7"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C7" s="5"/>
       <c r="E7"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="7"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C8" s="5"/>
       <c r="E8"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="7"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C9" s="5"/>
       <c r="E9"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="7"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C10" s="5"/>
       <c r="E10"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{1CE42BA1-3901-4634-AD9E-830522C582BA}"/>
   </hyperlinks>

</xml_diff>